<commit_message>
files added: Traceability Matrix Template (Requirements and testing), Design Specification Document Template (Conceptual design UML), Test plan
</commit_message>
<xml_diff>
--- a/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uidn8311\Desktop\Repositorios-GITHUB\V_cycle_proces\V-Cycle Process\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <sheet name="Module Verification" sheetId="4" r:id="rId5"/>
     <sheet name="SW Validation" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -321,7 +326,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -543,6 +548,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1738,7 +1746,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1773,7 +1781,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1984,9 +1992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -2000,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,9 +2231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
modified files: DSD and matrix
</commit_message>
<xml_diff>
--- a/V-Cycle Process/V_Cycle Process Script.xlsx
+++ b/V-Cycle Process/V_Cycle Process Script.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="2"/>
+    <workbookView xWindow="7890" yWindow="3180" windowWidth="15015" windowHeight="9330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="V-Cycle" sheetId="2" r:id="rId1"/>
@@ -2006,8 +2006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2231,8 +2231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:E27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>